<commit_message>
glances betareg models v2: change error in init-description
</commit_message>
<xml_diff>
--- a/data/processed/betareg_models_v2/glances.xlsx
+++ b/data/processed/betareg_models_v2/glances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ueli\Documents\myrepos\c3_analysis\data\processed\betareg_models_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87667A3-5482-4EEC-A1EA-3E7EB734A8E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C64DD73-54CC-46E0-BEE5-99616C173424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{E170DA96-0B14-455C-973A-0DE93C0492C3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{E170DA96-0B14-455C-973A-0DE93C0492C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -484,11 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3E1371C-EFDB-4768-B576-9BBFD649F899}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:N113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="G18" sqref="G18:G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -596,7 +595,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -640,7 +639,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -684,7 +683,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -728,7 +727,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -772,7 +771,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -816,7 +815,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -860,7 +859,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -904,7 +903,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -948,7 +947,7 @@
         <v>3456</v>
       </c>
     </row>
-    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -992,7 +991,7 @@
         <v>3456</v>
       </c>
     </row>
-    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1036,7 +1035,7 @@
         <v>3456</v>
       </c>
     </row>
-    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1080,7 +1079,7 @@
         <v>3456</v>
       </c>
     </row>
-    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1124,7 +1123,7 @@
         <v>3456</v>
       </c>
     </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1168,7 +1167,7 @@
         <v>3456</v>
       </c>
     </row>
-    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1212,7 +1211,7 @@
         <v>3456</v>
       </c>
     </row>
-    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1276,7 +1275,7 @@
         <v>21</v>
       </c>
       <c r="G18" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H18" s="1">
         <v>0.56123432318907895</v>
@@ -1320,7 +1319,7 @@
         <v>22</v>
       </c>
       <c r="G19" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H19" s="1">
         <v>0.66226816679505895</v>
@@ -1364,7 +1363,7 @@
         <v>23</v>
       </c>
       <c r="G20" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H20" s="1">
         <v>0.23921404068517799</v>
@@ -1408,7 +1407,7 @@
         <v>21</v>
       </c>
       <c r="G21" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H21" s="1">
         <v>0.56827822640640102</v>
@@ -1452,7 +1451,7 @@
         <v>22</v>
       </c>
       <c r="G22" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H22" s="1">
         <v>0.65052517697295198</v>
@@ -1496,7 +1495,7 @@
         <v>23</v>
       </c>
       <c r="G23" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H23" s="1">
         <v>0.27979559998418502</v>
@@ -1540,7 +1539,7 @@
         <v>21</v>
       </c>
       <c r="G24" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H24" s="1">
         <v>0.52782343891217098</v>
@@ -1584,7 +1583,7 @@
         <v>22</v>
       </c>
       <c r="G25" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H25" s="1">
         <v>0.401574265573374</v>
@@ -1628,7 +1627,7 @@
         <v>23</v>
       </c>
       <c r="G26" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H26" s="1">
         <v>0.64114161805636305</v>
@@ -1672,7 +1671,7 @@
         <v>21</v>
       </c>
       <c r="G27" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H27" s="1">
         <v>0.56064401076461501</v>
@@ -1716,7 +1715,7 @@
         <v>22</v>
       </c>
       <c r="G28" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H28" s="1">
         <v>0.58507763537899005</v>
@@ -1760,7 +1759,7 @@
         <v>23</v>
       </c>
       <c r="G29" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H29" s="1">
         <v>0.72085194482953197</v>
@@ -1804,7 +1803,7 @@
         <v>21</v>
       </c>
       <c r="G30" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H30" s="1">
         <v>0.433819411858679</v>
@@ -1848,7 +1847,7 @@
         <v>22</v>
       </c>
       <c r="G31" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H31" s="1">
         <v>0.62270601992646901</v>
@@ -1892,7 +1891,7 @@
         <v>23</v>
       </c>
       <c r="G32" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H32" s="1">
         <v>0.33472569057107898</v>
@@ -1936,7 +1935,7 @@
         <v>21</v>
       </c>
       <c r="G33" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H33" s="1">
         <v>0.44704369985068398</v>
@@ -1980,7 +1979,7 @@
         <v>22</v>
       </c>
       <c r="G34" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H34" s="1">
         <v>0.59867800806937699</v>
@@ -2024,7 +2023,7 @@
         <v>23</v>
       </c>
       <c r="G35" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H35" s="1">
         <v>0.65323969173808605</v>
@@ -2068,7 +2067,7 @@
         <v>21</v>
       </c>
       <c r="G36" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H36" s="1">
         <v>0.26888110499405898</v>
@@ -2112,7 +2111,7 @@
         <v>22</v>
       </c>
       <c r="G37" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H37" s="1">
         <v>0.41036207388594098</v>
@@ -2156,7 +2155,7 @@
         <v>23</v>
       </c>
       <c r="G38" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H38" s="1">
         <v>0.640499475420932</v>
@@ -2200,7 +2199,7 @@
         <v>21</v>
       </c>
       <c r="G39" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H39" s="1">
         <v>0.33611003699437503</v>
@@ -2244,7 +2243,7 @@
         <v>22</v>
       </c>
       <c r="G40" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H40" s="1">
         <v>0.41830727560593201</v>
@@ -2288,7 +2287,7 @@
         <v>23</v>
       </c>
       <c r="G41" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="H41" s="1">
         <v>0.72145049353802804</v>
@@ -5481,13 +5480,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N113" xr:uid="{A3E1371C-EFDB-4768-B576-9BBFD649F899}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="red"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:N113" xr:uid="{A3E1371C-EFDB-4768-B576-9BBFD649F899}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>